<commit_message>
duas opções de array
</commit_message>
<xml_diff>
--- a/Sensores_teste.xlsx
+++ b/Sensores_teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\P&amp;D\Grade-SAE\Sistema supervisório\teste_grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC02094-2A91-419D-B787-56F2C5C8D2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F796C4-0D42-4C40-B4D2-1A6B8BA868DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC8C4A39-25C0-4BB2-BEC4-3D28E2DBB0FB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Sensor</t>
   </si>
@@ -93,13 +93,19 @@
   </si>
   <si>
     <t>168-45</t>
+  </si>
+  <si>
+    <t>cte (um/m/°C)</t>
+  </si>
+  <si>
+    <t>T0 (°C)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +121,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,98 +143,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -233,35 +166,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B22B746-4F6A-427F-B759-EACDBF931EF2}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,197 +518,289 @@
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="1" customWidth="1"/>
-    <col min="5" max="9" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="9" width="12.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>1525.645</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="6">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="6">
         <v>30</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="6">
         <v>34.799999999999997</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="6">
         <v>-0.8</v>
       </c>
+      <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="6"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>1529.8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6">
         <v>0.76</v>
       </c>
       <c r="I3" s="6">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>30</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>1530.2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
         <v>0.79</v>
       </c>
       <c r="I4" s="6">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>30</v>
+      </c>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>1535.5519999999999</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>30</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>35.299999999999997</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="6">
         <v>-1</v>
       </c>
+      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="6"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>1540.2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
         <v>0.79</v>
       </c>
       <c r="I6" s="6">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="6">
         <v>1545.2719999999999</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>30</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="6">
         <v>34.6</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="6">
         <v>-0.7</v>
       </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="6">
         <v>1550.5</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>3</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6">
         <v>0.79</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="6">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
+        <v>30</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
   </sheetData>

</xml_diff>